<commit_message>
Gender added to sheet
</commit_message>
<xml_diff>
--- a/dg/media/data_upload/Sample_Person_Add.xlsx
+++ b/dg/media/data_upload/Sample_Person_Add.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Village_Name</t>
   </si>
@@ -34,6 +34,29 @@
   </si>
   <si>
     <t>Husband_Father_Surname</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Gender(M/F</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -383,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -394,9 +417,10 @@
     <col min="1" max="4" width="20.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="22.42578125" customWidth="1"/>
     <col min="6" max="6" width="24.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -415,24 +439,27 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>

</xml_diff>

<commit_message>
Age and phone number included in static  data upload. optional
</commit_message>
<xml_diff>
--- a/dg/media/data_upload/Sample_Person_Add.xlsx
+++ b/dg/media/data_upload/Sample_Person_Add.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Village_Name</t>
   </si>
@@ -57,6 +57,12 @@
       </rPr>
       <t>)</t>
     </r>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Phone_Number</t>
   </si>
 </sst>
 </file>
@@ -406,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,9 +424,10 @@
     <col min="5" max="5" width="22.42578125" customWidth="1"/>
     <col min="6" max="6" width="24.5703125" customWidth="1"/>
     <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -442,24 +449,30 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>

</xml_diff>